<commit_message>
excel utility implemented in login page
</commit_message>
<xml_diff>
--- a/RMGYantra/Resources/Data.xlsx
+++ b/RMGYantra/Resources/Data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\source\repos\RMGYantra\RMGYantra\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F538D62-65CA-4888-B1E2-93614B7E121E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24613530-2BB1-43AE-948B-80DE6A40A6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{03CAEEBD-3DD6-4205-AA01-0670E90A31AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{03CAEEBD-3DD6-4205-AA01-0670E90A31AD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PROJECTDATA" sheetId="1" r:id="rId1"/>
+    <sheet name="USERCREDENTIAL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>createdBy</t>
   </si>
@@ -70,16 +71,42 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>rmgy@9999</t>
+  </si>
+  <si>
+    <t>rmgyantra</t>
+  </si>
+  <si>
+    <t>http://localhost:8084/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,14 +129,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF218BF-49F7-47D3-BB1E-09DF9A15341F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,4 +519,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DF328F-56E6-41A7-AFC9-21C0AA1B2CB8}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{60B6913D-9C08-4530-A941-1F98C110BABA}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{46699151-F36F-4F41-B2B4-500709B250EC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
datadriven achieved for creating project
</commit_message>
<xml_diff>
--- a/RMGYantra/Resources/Data.xlsx
+++ b/RMGYantra/Resources/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\source\repos\RMGYantra\RMGYantra\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24613530-2BB1-43AE-948B-80DE6A40A6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD8A058-F152-4E98-8BEC-33D7E3020334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{03CAEEBD-3DD6-4205-AA01-0670E90A31AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{03CAEEBD-3DD6-4205-AA01-0670E90A31AD}"/>
   </bookViews>
   <sheets>
     <sheet name="PROJECTDATA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>createdBy</t>
   </si>
@@ -55,9 +55,6 @@
     <t>MediCare</t>
   </si>
   <si>
-    <t>OnGoging</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
@@ -89,6 +86,12 @@
   </si>
   <si>
     <t>http://localhost:8084/</t>
+  </si>
+  <si>
+    <t>On Goging</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -454,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF218BF-49F7-47D3-BB1E-09DF9A15341F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -496,24 +499,24 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -525,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2DF328F-56E6-41A7-AFC9-21C0AA1B2CB8}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -533,24 +536,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>